<commit_message>
Added config, added train, added test set
</commit_message>
<xml_diff>
--- a/time_logging.xlsx
+++ b/time_logging.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Philipp\Studium\11918494_nanoGPTQ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3C16D12-52DD-4ADC-BA09-BF21039C95E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7E795C1-E0D8-4D26-86CC-5399BB92DA0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3072" yWindow="3072" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="3">
   <si>
     <t>Setup</t>
   </si>
@@ -367,10 +367,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:F6"/>
+  <dimension ref="A2:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -417,7 +417,7 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="E3" s="2">
-        <f t="shared" ref="E3:E6" si="0">D3-C3</f>
+        <f t="shared" ref="E3:E8" si="0">D3-C3</f>
         <v>4.166666666666663E-2</v>
       </c>
       <c r="F3" t="s">
@@ -478,6 +478,42 @@
         <v>6.25E-2</v>
       </c>
       <c r="F6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B7" s="1">
+        <v>45972</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E7" s="2">
+        <f t="shared" si="0"/>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="F7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B8" s="1">
+        <v>45972</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.63888888888888884</v>
+      </c>
+      <c r="E8" s="2">
+        <f t="shared" si="0"/>
+        <v>1.388888888888884E-2</v>
+      </c>
+      <c r="F8" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Finished training script, train pipeline works
</commit_message>
<xml_diff>
--- a/time_logging.xlsx
+++ b/time_logging.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Philipp\Studium\11918494_nanoGPTQ\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phili\Documents\Master\11918494_nanoGPTQ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7E795C1-E0D8-4D26-86CC-5399BB92DA0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D53A1377-63EE-4D18-B324-3F932730A4D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3072" yWindow="3072" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="3">
   <si>
     <t>Setup</t>
   </si>
@@ -367,22 +368,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:F8"/>
+  <dimension ref="A2:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="8.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="8.1328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.1328125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
@@ -403,7 +404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>2</v>
       </c>
@@ -417,14 +418,14 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="E3" s="2">
-        <f t="shared" ref="E3:E8" si="0">D3-C3</f>
+        <f t="shared" ref="E3:E9" si="0">D3-C3</f>
         <v>4.166666666666663E-2</v>
       </c>
       <c r="F3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>3</v>
       </c>
@@ -445,7 +446,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B5" s="1">
         <v>45971</v>
       </c>
@@ -463,7 +464,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B6" s="1">
         <v>45971</v>
       </c>
@@ -481,7 +482,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B7" s="1">
         <v>45972</v>
       </c>
@@ -499,7 +500,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B8" s="1">
         <v>45972</v>
       </c>
@@ -514,6 +515,24 @@
         <v>1.388888888888884E-2</v>
       </c>
       <c r="F8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B9" s="1">
+        <v>45992</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0.71875</v>
+      </c>
+      <c r="E9" s="2">
+        <f t="shared" si="0"/>
+        <v>0.11458333333333337</v>
+      </c>
+      <c r="F9" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added sampling script, cleaned up config
</commit_message>
<xml_diff>
--- a/time_logging.xlsx
+++ b/time_logging.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phili\Documents\Master\11918494_nanoGPTQ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D53A1377-63EE-4D18-B324-3F932730A4D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82717F59-411F-46AF-9491-9C702922B89A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="3">
   <si>
     <t>Setup</t>
   </si>
@@ -368,7 +367,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:F9"/>
+  <dimension ref="A2:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
@@ -418,7 +417,7 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="E3" s="2">
-        <f t="shared" ref="E3:E9" si="0">D3-C3</f>
+        <f t="shared" ref="E3:E10" si="0">D3-C3</f>
         <v>4.166666666666663E-2</v>
       </c>
       <c r="F3" t="s">
@@ -533,6 +532,24 @@
         <v>0.11458333333333337</v>
       </c>
       <c r="F9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B10" s="1">
+        <v>45993</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="E10" s="2">
+        <f t="shared" si="0"/>
+        <v>9.375E-2</v>
+      </c>
+      <c r="F10" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Renamed checkpoints, added naive quant
</commit_message>
<xml_diff>
--- a/time_logging.xlsx
+++ b/time_logging.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phili\Documents\Master\11918494_nanoGPTQ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82717F59-411F-46AF-9491-9C702922B89A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AF6F6BA-5C00-4910-BA5F-3958222B14D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="368" yWindow="368" windowWidth="16199" windowHeight="9847" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="5">
   <si>
     <t>Setup</t>
   </si>
@@ -45,6 +45,12 @@
   </si>
   <si>
     <t>NanoGPT</t>
+  </si>
+  <si>
+    <t>Baseline Training</t>
+  </si>
+  <si>
+    <t>Naive Quantization</t>
   </si>
 </sst>
 </file>
@@ -367,10 +373,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:F10"/>
+  <dimension ref="A2:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -417,7 +423,7 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="E3" s="2">
-        <f t="shared" ref="E3:E10" si="0">D3-C3</f>
+        <f t="shared" ref="E3:E13" si="0">D3-C3</f>
         <v>4.166666666666663E-2</v>
       </c>
       <c r="F3" t="s">
@@ -551,6 +557,60 @@
       </c>
       <c r="F10" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B11" s="1">
+        <v>45993</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1</v>
+      </c>
+      <c r="E11" s="2">
+        <f t="shared" si="0"/>
+        <v>0.375</v>
+      </c>
+      <c r="F11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B12" s="1">
+        <v>45995</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0.46875</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0.53125</v>
+      </c>
+      <c r="E12" s="2">
+        <f t="shared" si="0"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="F12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B13" s="1">
+        <v>45995</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0.59375</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="E13" s="2">
+        <f t="shared" si="0"/>
+        <v>1.041666666666663E-2</v>
+      </c>
+      <c r="F13" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added tests and typechecking
</commit_message>
<xml_diff>
--- a/time_logging.xlsx
+++ b/time_logging.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phili\Documents\Master\11918494_nanoGPTQ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D957C888-F6B5-4C33-8886-B79B1A26F699}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8F473BB-E844-4059-A7E1-09E7BE59CD07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1103" yWindow="1103" windowWidth="16200" windowHeight="9847" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2093" yWindow="577" windowWidth="16200" windowHeight="9848" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="7">
   <si>
     <t>Setup</t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>GPTQ</t>
+  </si>
+  <si>
+    <t>Evaluate Models</t>
   </si>
 </sst>
 </file>
@@ -376,10 +379,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:F15"/>
+  <dimension ref="A2:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -426,7 +429,7 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="E3" s="2">
-        <f t="shared" ref="E3:E15" si="0">D3-C3</f>
+        <f t="shared" ref="E3:E16" si="0">D3-C3</f>
         <v>4.166666666666663E-2</v>
       </c>
       <c r="F3" t="s">
@@ -650,6 +653,32 @@
       </c>
       <c r="F15" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B16" s="1">
+        <v>45999</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0.63541666666666663</v>
+      </c>
+      <c r="E16" s="2">
+        <f t="shared" si="0"/>
+        <v>0.125</v>
+      </c>
+      <c r="F16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B17" s="1">
+        <v>45999</v>
+      </c>
+      <c r="F17" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added function and class docstrings
</commit_message>
<xml_diff>
--- a/time_logging.xlsx
+++ b/time_logging.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phili\Documents\Master\11918494_nanoGPTQ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8F473BB-E844-4059-A7E1-09E7BE59CD07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0B98490-CE3E-45CB-AD09-85FE55EDA419}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2093" yWindow="577" windowWidth="16200" windowHeight="9848" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -382,7 +382,7 @@
   <dimension ref="A2:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -677,6 +677,9 @@
       <c r="B17" s="1">
         <v>45999</v>
       </c>
+      <c r="C17" s="2">
+        <v>0.47916666666666669</v>
+      </c>
       <c r="F17" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
Added evaluation, changed dataset to tinystories
</commit_message>
<xml_diff>
--- a/time_logging.xlsx
+++ b/time_logging.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phili\Documents\Master\11918494_nanoGPTQ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0B98490-CE3E-45CB-AD09-85FE55EDA419}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24E9C72A-87B9-48C7-AAC3-8CA0E5D5425E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2093" yWindow="577" windowWidth="16200" windowHeight="9848" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="7">
   <si>
     <t>Setup</t>
   </si>
@@ -379,10 +379,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:F17"/>
+  <dimension ref="A2:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -429,7 +429,7 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="E3" s="2">
-        <f t="shared" ref="E3:E16" si="0">D3-C3</f>
+        <f t="shared" ref="E3:E18" si="0">D3-C3</f>
         <v>4.166666666666663E-2</v>
       </c>
       <c r="F3" t="s">
@@ -680,8 +680,44 @@
       <c r="C17" s="2">
         <v>0.47916666666666669</v>
       </c>
+      <c r="D17" s="2">
+        <v>0.59375</v>
+      </c>
+      <c r="E17" s="2">
+        <f t="shared" si="0"/>
+        <v>0.11458333333333331</v>
+      </c>
       <c r="F17" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B18" s="1">
+        <v>45999</v>
+      </c>
+      <c r="C18" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="E18" s="2">
+        <f t="shared" si="0"/>
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="F18" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B19" s="1">
+        <v>45999</v>
+      </c>
+      <c r="C19" s="2">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="F19" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added demo and tests
</commit_message>
<xml_diff>
--- a/time_logging.xlsx
+++ b/time_logging.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phili\Documents\Master\11918494_nanoGPTQ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24E9C72A-87B9-48C7-AAC3-8CA0E5D5425E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EEA3C27-3439-47DA-AECD-F8B65F24FBA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2093" yWindow="577" windowWidth="16200" windowHeight="9848" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="8">
   <si>
     <t>Setup</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>Evaluate Models</t>
+  </si>
+  <si>
+    <t>Demo</t>
   </si>
 </sst>
 </file>
@@ -379,10 +382,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:F19"/>
+  <dimension ref="A2:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -429,7 +432,7 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="E3" s="2">
-        <f t="shared" ref="E3:E18" si="0">D3-C3</f>
+        <f t="shared" ref="E3:E20" si="0">D3-C3</f>
         <v>4.166666666666663E-2</v>
       </c>
       <c r="F3" t="s">
@@ -716,8 +719,33 @@
       <c r="C19" s="2">
         <v>0.64583333333333337</v>
       </c>
+      <c r="D19" s="2">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="E19" s="2">
+        <f t="shared" si="0"/>
+        <v>8.3333333333333259E-2</v>
+      </c>
       <c r="F19" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B20" s="1">
+        <v>45999</v>
+      </c>
+      <c r="C20" s="2">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="D20" s="2">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="E20" s="2">
+        <f t="shared" si="0"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="F20" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed src module and improved readme
</commit_message>
<xml_diff>
--- a/time_logging.xlsx
+++ b/time_logging.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phili\Documents\Master\11918494_nanoGPTQ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EEA3C27-3439-47DA-AECD-F8B65F24FBA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF3E5F8A-C499-4DB6-949E-4094E0A56F42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-17415" yWindow="195" windowWidth="16200" windowHeight="9855" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -384,8 +384,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -522,11 +522,11 @@
         <v>0.625</v>
       </c>
       <c r="D8" s="2">
-        <v>0.63888888888888884</v>
+        <v>0.64583333333333337</v>
       </c>
       <c r="E8" s="2">
         <f t="shared" si="0"/>
-        <v>1.388888888888884E-2</v>
+        <v>2.083333333333337E-2</v>
       </c>
       <c r="F8" t="s">
         <v>2</v>
@@ -612,11 +612,11 @@
         <v>0.59375</v>
       </c>
       <c r="D13" s="2">
-        <v>0.60416666666666663</v>
+        <v>0.61458333333333337</v>
       </c>
       <c r="E13" s="2">
         <f t="shared" si="0"/>
-        <v>1.041666666666663E-2</v>
+        <v>2.083333333333337E-2</v>
       </c>
       <c r="F13" t="s">
         <v>4</v>
@@ -684,11 +684,11 @@
         <v>0.47916666666666669</v>
       </c>
       <c r="D17" s="2">
-        <v>0.59375</v>
+        <v>0.60416666666666663</v>
       </c>
       <c r="E17" s="2">
         <f t="shared" si="0"/>
-        <v>0.11458333333333331</v>
+        <v>0.12499999999999994</v>
       </c>
       <c r="F17" t="s">
         <v>6</v>

</xml_diff>